<commit_message>
ENH: return an OrderedDict from read_excel with sheetname=None
</commit_message>
<xml_diff>
--- a/pandas/io/tests/data/test_multisheet.xlsx
+++ b/pandas/io/tests/data/test_multisheet.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Desktop\Projects\opensheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21420" windowHeight="12030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21420" windowHeight="12040"/>
   </bookViews>
   <sheets>
-    <sheet name="Alpha" sheetId="1" r:id="rId1"/>
-    <sheet name="Beta" sheetId="2" r:id="rId2"/>
-    <sheet name="Charlie" sheetId="3" r:id="rId3"/>
+    <sheet name="Charlie" sheetId="3" r:id="rId1"/>
+    <sheet name="Alpha" sheetId="1" r:id="rId2"/>
+    <sheet name="Beta" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -136,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -171,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -358,16 +356,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -381,115 +379,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <f>DATE(2014,1,1)</f>
-        <v>41640</v>
+        <f>DATE(2014,3,15)</f>
+        <v>41713</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>B2+1</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <f>C2+1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <f>A2+1</f>
-        <v>41641</v>
+        <v>41714</v>
       </c>
       <c r="B3">
         <f>B2+1</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:D7" si="0">B3+1</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A7" si="1">A3+1</f>
-        <v>41642</v>
+        <f t="shared" ref="A4:B7" si="1">A3+1</f>
+        <v>41715</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B7" si="2">B3+1</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
-        <v>41643</v>
+        <v>41716</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
-        <v>41644</v>
+        <v>41717</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
-        <v>41645</v>
+        <v>41718</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -498,15 +501,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D7" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -520,10 +523,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <f>DATE(2014,6,1)</f>
-        <v>41791</v>
+        <f>DATE(2014,1,1)</f>
+        <v>41640</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -537,10 +540,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <f>A2+1</f>
-        <v>41792</v>
+        <v>41641</v>
       </c>
       <c r="B3">
         <f>B2+1</f>
@@ -555,13 +558,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:B7" si="1">A3+1</f>
-        <v>41793</v>
+        <f t="shared" ref="A4:A7" si="1">A3+1</f>
+        <v>41642</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B4:B7" si="2">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4">
@@ -573,13 +576,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
-        <v>41794</v>
+        <v>41643</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C5">
@@ -591,13 +594,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
-        <v>41795</v>
+        <v>41644</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C6">
@@ -609,13 +612,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
-        <v>41796</v>
+        <v>41645</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C7">
@@ -629,6 +632,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -636,16 +644,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -659,114 +667,119 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <f>DATE(2014,3,15)</f>
-        <v>41713</v>
+        <f>DATE(2014,6,1)</f>
+        <v>41791</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>B2+1</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <f>C2+1</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <f>A2+1</f>
-        <v>41714</v>
+        <v>41792</v>
       </c>
       <c r="B3">
         <f>B2+1</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:D7" si="0">B3+1</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <f t="shared" ref="A4:B7" si="1">A3+1</f>
-        <v>41715</v>
+        <v>41793</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
-        <v>41716</v>
+        <v>41794</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
-        <v>41717</v>
+        <v>41795</v>
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
-        <v>41718</v>
+        <v>41796</v>
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>